<commit_message>
GeoHash test with BPC(2 method)
</commit_message>
<xml_diff>
--- a/LabReport/Lab3/Lab3 (Graph Coverage  test case design)1.xlsx
+++ b/LabReport/Lab3/Lab3 (Graph Coverage  test case design)1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HongDeLiu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HongDeLiu\Desktop\GeoProject\LabReport\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDE22B6-C979-4400-AF9B-E722027B58D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD048C6-EEE8-4FFF-849E-F5F91F73639B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
   <si>
     <t>Method</t>
   </si>
@@ -323,6 +323,168 @@
   </si>
   <si>
     <t>n/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">        checkHash(hash);
+        Preconditions.checkArgument(hash.length() &gt; 0,
+                "adjacent has no meaning for a zero length hash that covers the whole world");
+        String adjacentHashAtBorder = adjacentHashAtBorder(hash, direction);
+        if (adjacentHashAtBorder != null)
+            return adjacentHashAtBorder;
+        String source = hash.toLowerCase();
+        char lastChar = source.charAt(source.length() - 1);
+        Parity parity = (source.length() % 2 == 0) ? Parity.EVEN : Parity.ODD;
+        String base = source.substring(0, source.length() - 1);
+        if (BORDERS.get(direction).get(parity).indexOf(lastChar) != -1)
+            base = adjacentHash(base, direction);
+        return base + BASE32.charAt(NEIGHBOURS.get(direction).get(parity).indexOf(lastChar));</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1, 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3, 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adjacentHash(String hash, Direction direction)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GeoHash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：String hash
+2：Direction direction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the adjacent hash in given</t>
+  </si>
+  <si>
+    <t>adjacentHash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adjacentHash_CFG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1：{1, 3, 5, 6, 8, 9, 10, 11}
+P2：{1, 3, 5, 6, 8, 9, 11}
+P3：{1, 3, 5, 6, 7}
+P4：{1, 3, 4}
+P5：{1, 2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{P1, P2, P3, P4, P5}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{hash="2b", direction=RIGHT; expected="30"}
+T2：{hash="11", direction=RIGHT; expected="13"}
+T3：{hash="x", direction=RIGHT; expected="8"}
+T4：{hash="", direction=RIGHT; expected=IllegalArgumentException}
+T5：{hash=null, direction=RIGHT;expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers P1{1, 3, 5, 6, 8, 9, 10, 11}
+T2 covers P2{1, 3, 5, 6, 8, 9, 11}
+T3 covers P3{1, 3, 5, 6, 7}
+T4 covers P4{1, 3, 4}
+T5 covers P5{1, 2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adjacentHash(String hash, Direction direction, int steps)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：String hash
+2：Direction direction
+3：int steps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the adjacent hash N steps in the given.
+A negative N will use the opposite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (steps &lt; 0)
+            return adjacentHash(hash, direction.opposite(), Math.abs(steps));
+        else {
+            String h = hash;
+            for (int i = 0; i &lt; steps; i++)
+                h = adjacentHash(h, direction);
+            return h;
+        }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4, 5, 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6, 7, 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adjacentHash_step</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adjacentHash_step_CFG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1：{1, 2, 1, 3, 4, 5, 8, 9, 5, 10}
+P2：{1, 2, 1, 3, 4, 5, 6}
+P3：{1, 2, 1, 3, 4, 5, 7}
+P4：{1, 2, 1, 3, 4, 5, 10}
+P5：{1, 3, 4, 5, 6}
+P6：{1, 3, 4, 5, 7}
+P7：{1, 3, 4, 5, 10}
+P8：{1, 3, 4, 5, 8, 9, 5, 10}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P4：{1, 2, 1, 3, 4, 5, 10}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P4：{1, 2, 1, 3, 4, 5, 8, 9, 5, 10}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{P4, P5, P6, P7, P8}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{hash="2b", direction=LEFT, stpes=-1; expected="30"}
+T2：{hash="", direction=LEFT, steps=1; expected=IllegalArgumentException}
+T3：{hash=null, direction=LEFT, steps=1; expected=IllegalArgumentException}
+T4：{hash="2b", direction=LEFT, steps=0; expected="2b"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers P4,P8{1, 2, 1, 3, 4, 5, 8, 9, 5, 10}
+T2 covers P5{1, 3, 4, 5, 6}
+T3 covers P6{1, 3, 4, 5, 7}
+T4 covers P7{1, 3, 4, 5, 10}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -497,7 +659,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -546,6 +708,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,8 +738,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
@@ -573,8 +759,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -688,6 +880,106 @@
         <a:xfrm>
           <a:off x="6720841" y="5173980"/>
           <a:ext cx="3706340" cy="3878580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>205739</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>110010</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="圖片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7AF4BA8-AC36-4849-84A8-FCAD544998C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8549640" y="10340339"/>
+          <a:ext cx="3649980" cy="4636291"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>23494</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="圖片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E6318EC-29EE-49A5-9894-33EEC7CC112A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6720840" y="16512540"/>
+          <a:ext cx="3642360" cy="4755514"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -962,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1042,7 +1334,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="97.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -1086,7 +1378,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="113.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
@@ -1098,10 +1390,10 @@
       <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="17" t="s">
         <v>42</v>
       </c>
       <c r="G3" s="13" t="s">
@@ -1110,7 +1402,7 @@
       <c r="H3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="18" t="s">
         <v>46</v>
       </c>
       <c r="L3" t="s">
@@ -1119,14 +1411,102 @@
       <c r="M3" t="s">
         <v>49</v>
       </c>
-      <c r="N3" s="23" t="s">
+      <c r="N3" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="18" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="243" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="226.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" t="s">
+        <v>74</v>
+      </c>
+      <c r="N5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="35" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1136,6 +1516,10 @@
     <hyperlink ref="H2" location="'code and graph'!L1" display="encodeBase32_CFG" xr:uid="{93818865-5FAE-4C11-B7B0-24BF9760B189}"/>
     <hyperlink ref="G3" location="'code and graph'!A38" display="decodeBase32" xr:uid="{F85B5F0E-FDEE-434F-9054-911B46DD71E0}"/>
     <hyperlink ref="H3" location="'code and graph'!L38" display="decoeBase32_CFG" xr:uid="{1AAD3334-C1A6-4BB4-B21A-F243C35ED1C3}"/>
+    <hyperlink ref="G4" location="'code and graph'!A66" display="adjacentHash" xr:uid="{C7B464B2-DF37-4452-BD4D-DB033C968627}"/>
+    <hyperlink ref="H4" location="'code and graph'!O66" display="adjacentHash_CFG" xr:uid="{58CC51C5-926D-43D9-B92A-D4BA0B15BB36}"/>
+    <hyperlink ref="G5" location="'code and graph'!A89" display="adjacentHash_step" xr:uid="{8CC4F788-459E-4021-A51A-8AED32F1CFAA}"/>
+    <hyperlink ref="H5" location="'code and graph'!L95" display="adjacentHash_step_CFG" xr:uid="{60D699C3-C2AC-4C76-A8E0-007C11D319EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1144,10 +1528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8F8B7E-6CC2-472A-ADFE-A1AB13588D91}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="T41" sqref="T41"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="L95" sqref="L95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1159,15 +1543,15 @@
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="10" t="s">
         <v>25</v>
       </c>
@@ -1176,16 +1560,16 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="20">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="24">
         <v>1</v>
       </c>
     </row>
@@ -1193,39 +1577,39 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
       <c r="I5" s="11">
         <v>2</v>
       </c>
@@ -1234,13 +1618,13 @@
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="11">
         <v>3</v>
       </c>
@@ -1249,13 +1633,13 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="11">
         <v>4</v>
       </c>
@@ -1264,14 +1648,14 @@
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="20">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="24">
         <v>5</v>
       </c>
     </row>
@@ -1279,40 +1663,40 @@
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="20">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="24">
         <v>6</v>
       </c>
     </row>
@@ -1320,37 +1704,37 @@
       <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="24"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
       <c r="I14" s="11">
         <v>7</v>
       </c>
@@ -1359,13 +1743,13 @@
       <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
       <c r="I15" s="11">
         <v>8</v>
       </c>
@@ -1374,26 +1758,26 @@
       <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
       <c r="I16" s="11"/>
     </row>
     <row r="17" spans="1:9" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
       <c r="I17" s="12">
         <v>9</v>
       </c>
@@ -1404,15 +1788,15 @@
       <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="10" t="s">
         <v>25</v>
       </c>
@@ -1421,16 +1805,16 @@
       <c r="A27" s="8">
         <v>1</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="20">
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="24">
         <v>1</v>
       </c>
     </row>
@@ -1438,52 +1822,52 @@
       <c r="A28" s="8">
         <v>2</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="20"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="24"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>3</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="20"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="24"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>4</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="20"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="24"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>5</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
       <c r="I31" s="11" t="s">
         <v>36</v>
       </c>
@@ -1492,13 +1876,13 @@
       <c r="A32" s="8">
         <v>6</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
       <c r="I32" s="11" t="s">
         <v>37</v>
       </c>
@@ -1507,14 +1891,14 @@
       <c r="A33" s="8">
         <v>7</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="20">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="24">
         <v>6</v>
       </c>
     </row>
@@ -1522,39 +1906,39 @@
       <c r="A34" s="8">
         <v>8</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="20"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="24"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>9</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="20"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="24"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>10</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
       <c r="I36" s="11">
         <v>8</v>
       </c>
@@ -1563,13 +1947,13 @@
       <c r="A37" s="8">
         <v>11</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
       <c r="I37" s="11">
         <v>9</v>
       </c>
@@ -1578,20 +1962,434 @@
       <c r="A38" s="9">
         <v>12</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
       <c r="I38" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="16.8" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="26">
+        <v>2</v>
+      </c>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="30"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="26"/>
+      <c r="L55" s="29"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>5</v>
+      </c>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26"/>
+      <c r="L58" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="29"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>6</v>
+      </c>
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="26"/>
+      <c r="L60" s="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>7</v>
+      </c>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="26"/>
+      <c r="L61" s="30"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>8</v>
+      </c>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="30"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>9</v>
+      </c>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="26"/>
+      <c r="J63" s="26"/>
+      <c r="K63" s="26"/>
+      <c r="L63" s="30"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>10</v>
+      </c>
+      <c r="B64" s="26"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="26"/>
+      <c r="I64" s="26"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="26"/>
+      <c r="L64" s="29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>11</v>
+      </c>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="26"/>
+      <c r="J65" s="26"/>
+      <c r="K65" s="26"/>
+      <c r="L65" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>12</v>
+      </c>
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="26"/>
+      <c r="H66" s="26"/>
+      <c r="I66" s="26"/>
+      <c r="J66" s="26"/>
+      <c r="K66" s="26"/>
+      <c r="L66" s="29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B81" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C81" s="30"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="30"/>
+      <c r="G81" s="30"/>
+      <c r="H81" s="30"/>
+      <c r="I81" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>1</v>
+      </c>
+      <c r="B82" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="26"/>
+      <c r="G82" s="26"/>
+      <c r="H82" s="26"/>
+      <c r="I82" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>2</v>
+      </c>
+      <c r="B83" s="26"/>
+      <c r="C83" s="26"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="26"/>
+      <c r="G83" s="26"/>
+      <c r="H83" s="26"/>
+      <c r="I83" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>3</v>
+      </c>
+      <c r="B84" s="26"/>
+      <c r="C84" s="26"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="26"/>
+      <c r="G84" s="26"/>
+      <c r="H84" s="26"/>
+      <c r="I84" s="29"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>4</v>
+      </c>
+      <c r="B85" s="26"/>
+      <c r="C85" s="26"/>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="26"/>
+      <c r="G85" s="26"/>
+      <c r="H85" s="26"/>
+      <c r="I85" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>5</v>
+      </c>
+      <c r="B86" s="26"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="26"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="26"/>
+      <c r="I86" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>6</v>
+      </c>
+      <c r="B87" s="26"/>
+      <c r="C87" s="26"/>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="26"/>
+      <c r="G87" s="26"/>
+      <c r="H87" s="26"/>
+      <c r="I87" s="29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>7</v>
+      </c>
+      <c r="B88" s="26"/>
+      <c r="C88" s="26"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="26"/>
+      <c r="G88" s="26"/>
+      <c r="H88" s="26"/>
+      <c r="I88" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>8</v>
+      </c>
+      <c r="B89" s="26"/>
+      <c r="C89" s="26"/>
+      <c r="D89" s="26"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="26"/>
+      <c r="G89" s="26"/>
+      <c r="H89" s="26"/>
+      <c r="I89" s="29"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="16">
+    <mergeCell ref="B82:H89"/>
+    <mergeCell ref="B81:H81"/>
+    <mergeCell ref="B52:K66"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="L60:L63"/>
+    <mergeCell ref="B51:K51"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B27:H38"/>
     <mergeCell ref="B26:H26"/>

</xml_diff>

<commit_message>
Base32 test with BPC complete and few test in other class
</commit_message>
<xml_diff>
--- a/LabReport/Lab3/Lab3 (Graph Coverage  test case design)1.xlsx
+++ b/LabReport/Lab3/Lab3 (Graph Coverage  test case design)1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HongDeLiu\Desktop\GeoProject\LabReport\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD048C6-EEE8-4FFF-849E-F5F91F73639B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC752D2-A8A6-4B14-855A-F8E4183D1313}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="129">
   <si>
     <t>Method</t>
   </si>
@@ -485,6 +485,246 @@
 T2 covers P5{1, 3, 4, 5, 6}
 T3 covers P6{1, 3, 4, 5, 7}
 T4 covers P7{1, 3, 4, 5, 10}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>encodeHash(double latitude, double longitude, int length)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：double latitude
+2：double latitude
+3：int length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return a geohash of with given length for the given latitude and longitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">        Preconditions.checkArgument(length &gt; 0, "length must be greater than zero");
+        Preconditions.checkArgument(latitude &gt;= -90 &amp;&amp; latitude &lt;= 90,
+                "latitude must be between -90 and 90 inclusive");
+        longitude = Position.to180(longitude);
+        return fromLongToString(encodeHashToLong(latitude, longitude, length));</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1, 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3, 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6, 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>encodeHash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>encodeHash_CFG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1：{1, 3, 5, 7}
+P2：{1, 3, 5, 6}
+P3：{1, 3, 4}
+P4：{1, 2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{P1, P2, P3, P4}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{latitude=90, longitude=90, length=3; expected="ypb"}
+T2：{latitude=90, longitude=90, length=13; expected=IllegalArgumentException}
+T3：{latitude=91, longitude=90, length=3; expected=IllegalArgumentException}
+T4：{latitude=90, longitude=90, length=-1; expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers P1{1, 3, 5, 7}
+T2 covers P2{1, 3, 5, 6}
+T3 covers P3{1, 3, 4}
+T4 covers P4{1, 2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CoverageLongs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getHashLength</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getHashLength()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>build CoverageLongs object first
+1. long[] hashes
+2. int count
+3. double ratio</t>
+  </si>
+  <si>
+    <t>int result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the length in characters of the first hash returned by an iterator on the hash set.</t>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (count == 0)
+            return 0;
+        else
+            return (int) (hashes[0] &amp; 0x0f);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getHashLength_CFG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1：{1, 2}
+P2：{1, 3}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{P1, P2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{CoverageLongs(hashes=[5, 9, 1], count=0, ratio=1.1); expected=0}
+T2：{CoverageLongs(hashes=[5, 9, 1], count=1, ratio=1.1); expected=5}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers P1{1, 2}
+T2 covers P2{1, 3}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getCharIndex(char ch)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：char ch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return index of the character in characterIndexes map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Integer result = characterIndexes.get(ch);
+        if (result == null)
+            throw new IllegalArgumentException("not a base32 character: " + ch);
+        else
+            return result;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getCharIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getCharIndex_CFG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1：{1, 2, 3}
+P2：{1, 2, 4}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{ch='a'; expected=IllegalArgumentException}
+T2：{ch='b'; expected=10}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers P1{1, 2, 3}
+T2 covers P2{1, 2, 4}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>padLeftWithZerosToLength(String s, int length)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：String s
+2：int length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return padded string with left zeros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (s.length() &lt; length) {
+            int count = length - s.length();
+            StringBuilder b = new StringBuilder();
+            for (int i = 0; i &lt; count; i++)
+                b.append('0');
+            b.append(s);
+            return b.toString();
+        } else
+            return s;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3, 4, 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>padLeftWithZerosToLength</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>padLeftWithZerosToLength_CFG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1：{1, 2, 3, 4, 5, 6, 4, 7}
+P2：{1, 2, 3, 4, 7}
+P3：{1, 8}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{P1, P2, P3}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2{1, 2, 3, 4, 7}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2{1, 2, 3, 4, 5, 6, 4, 7}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{s="1", length=2; expected="01"}
+T2：{s="11", length=1; expected="11"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers P1,P2{1, 2, 3, 4, 5, 6, 4, 7}
+T2 covers P3{1, 8}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -659,7 +899,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -720,6 +960,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -738,28 +996,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -899,7 +1154,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>601980</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>110010</xdr:rowOff>
+      <xdr:rowOff>79530</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -949,7 +1204,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>594360</xdr:colOff>
       <xdr:row>103</xdr:row>
-      <xdr:rowOff>23494</xdr:rowOff>
+      <xdr:rowOff>634</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -980,6 +1235,206 @@
         <a:xfrm>
           <a:off x="6720840" y="16512540"/>
           <a:ext cx="3642360" cy="4755514"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>603749</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="圖片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D856C074-EE7C-436A-BF35-920660A69A2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7330440" y="22745700"/>
+          <a:ext cx="3651749" cy="2865120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>592455</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="圖片 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{774A4FC9-EF29-45B1-B526-DEDA8A9D334C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4892040" y="26898600"/>
+          <a:ext cx="3030855" cy="1310640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>22861</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>151146</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="圖片 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB5A7DC0-C426-4C9D-AA96-24DA55385EA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7330441" y="28978860"/>
+          <a:ext cx="3680460" cy="2231406"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>88919</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="圖片 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CE9992B-4626-46CD-AA96-7CA0A669A251}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5501640" y="32095440"/>
+          <a:ext cx="3634740" cy="5461019"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1254,29 +1709,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375"/>
-    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" customWidth="1"/>
-    <col min="8" max="8" width="25.21875" customWidth="1"/>
-    <col min="9" max="9" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="65.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="18.6640625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" customWidth="1"/>
-    <col min="13" max="13" width="21.77734375" customWidth="1"/>
-    <col min="14" max="14" width="26.109375" customWidth="1"/>
-    <col min="15" max="15" width="29" customWidth="1"/>
-    <col min="16" max="16" width="17.88671875" customWidth="1"/>
+    <col min="12" max="12" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.88671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1434,10 +1889,10 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="13" t="s">
@@ -1452,10 +1907,10 @@
       <c r="L4" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="31" t="s">
+      <c r="M4" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="31" t="s">
+      <c r="N4" s="21" t="s">
         <v>49</v>
       </c>
       <c r="O4" s="18" t="s">
@@ -1466,31 +1921,31 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="226.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="23" t="s">
         <v>71</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="25" t="s">
         <v>73</v>
       </c>
       <c r="L5" t="s">
@@ -1502,11 +1957,187 @@
       <c r="N5" t="s">
         <v>75</v>
       </c>
-      <c r="O5" s="35" t="s">
+      <c r="O5" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="25" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="226.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="L6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="P6" s="33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="113.4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" t="s">
+        <v>104</v>
+      </c>
+      <c r="M7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="P7" s="36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="P8" s="38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I9" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="L9" t="s">
+        <v>124</v>
+      </c>
+      <c r="M9" t="s">
+        <v>125</v>
+      </c>
+      <c r="N9" t="s">
+        <v>126</v>
+      </c>
+      <c r="O9" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="P9" s="40" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1520,6 +2151,14 @@
     <hyperlink ref="H4" location="'code and graph'!O66" display="adjacentHash_CFG" xr:uid="{58CC51C5-926D-43D9-B92A-D4BA0B15BB36}"/>
     <hyperlink ref="G5" location="'code and graph'!A89" display="adjacentHash_step" xr:uid="{8CC4F788-459E-4021-A51A-8AED32F1CFAA}"/>
     <hyperlink ref="H5" location="'code and graph'!L95" display="adjacentHash_step_CFG" xr:uid="{60D699C3-C2AC-4C76-A8E0-007C11D319EF}"/>
+    <hyperlink ref="G6" location="'code and graph'!A117" display="encodeHash" xr:uid="{D6287632-8366-4EE2-92B9-7797E040AA02}"/>
+    <hyperlink ref="H6" location="'code and graph'!M124" display="encodeHash_CFG" xr:uid="{67AF9814-11A0-45DF-8661-D0436F925801}"/>
+    <hyperlink ref="G7" location="'code and graph'!A135" display="getHashLength" xr:uid="{CA366729-C650-4D38-B591-1EDC8252D7BA}"/>
+    <hyperlink ref="H7" location="'code and graph'!I135" display="getHashLength_CFG" xr:uid="{866D8693-0BA2-44E1-B967-8C673C234DCE}"/>
+    <hyperlink ref="G8" location="'code and graph'!A146" display="getCharIndex" xr:uid="{8683E2F3-5B45-4AA3-8B34-C39697AD5846}"/>
+    <hyperlink ref="H8" location="'code and graph'!M150" display="getCharIndex_CFG" xr:uid="{70F7C54B-4DA1-4782-ABDE-AE5069B13DB3}"/>
+    <hyperlink ref="G9" location="'code and graph'!A165" display="padLeftWithZerosToLength" xr:uid="{0BED5304-C8EE-47F9-A348-EAB25F91E807}"/>
+    <hyperlink ref="H9" location="'code and graph'!J175" display="padLeftWithZerosToLength_CFG" xr:uid="{7CA628C3-BCDB-41F6-BF99-290C634955FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1528,10 +2167,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8F8B7E-6CC2-472A-ADFE-A1AB13588D91}">
-  <dimension ref="A1:L89"/>
+  <dimension ref="A1:L166"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="L95" sqref="L95"/>
+    <sheetView topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="J175" sqref="J175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1543,15 +2182,15 @@
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
       <c r="I1" s="10" t="s">
         <v>25</v>
       </c>
@@ -1560,16 +2199,16 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="24">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="30">
         <v>1</v>
       </c>
     </row>
@@ -1577,39 +2216,39 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="24"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="24"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
       <c r="I5" s="11">
         <v>2</v>
       </c>
@@ -1618,13 +2257,13 @@
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
       <c r="I6" s="11">
         <v>3</v>
       </c>
@@ -1633,13 +2272,13 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="11">
         <v>4</v>
       </c>
@@ -1648,14 +2287,14 @@
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="24">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="30">
         <v>5</v>
       </c>
     </row>
@@ -1663,40 +2302,40 @@
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="24"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="24"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="30"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="24">
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="30">
         <v>6</v>
       </c>
     </row>
@@ -1704,37 +2343,37 @@
       <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="24"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="30"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="24"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="30"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
       <c r="I14" s="11">
         <v>7</v>
       </c>
@@ -1743,13 +2382,13 @@
       <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
       <c r="I15" s="11">
         <v>8</v>
       </c>
@@ -1758,26 +2397,26 @@
       <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
       <c r="I16" s="11"/>
     </row>
     <row r="17" spans="1:9" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
       <c r="I17" s="12">
         <v>9</v>
       </c>
@@ -1788,15 +2427,15 @@
       <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
       <c r="I26" s="10" t="s">
         <v>25</v>
       </c>
@@ -1805,16 +2444,16 @@
       <c r="A27" s="8">
         <v>1</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="24">
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="30">
         <v>1</v>
       </c>
     </row>
@@ -1822,52 +2461,52 @@
       <c r="A28" s="8">
         <v>2</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="24"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="30"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>3</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="24"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="30"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>4</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="24"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="30"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>5</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
       <c r="I31" s="11" t="s">
         <v>36</v>
       </c>
@@ -1876,13 +2515,13 @@
       <c r="A32" s="8">
         <v>6</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
       <c r="I32" s="11" t="s">
         <v>37</v>
       </c>
@@ -1891,14 +2530,14 @@
       <c r="A33" s="8">
         <v>7</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="24">
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="30">
         <v>6</v>
       </c>
     </row>
@@ -1906,39 +2545,39 @@
       <c r="A34" s="8">
         <v>8</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="24"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="30"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>9</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="24"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="30"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>10</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
       <c r="I36" s="11">
         <v>8</v>
       </c>
@@ -1947,13 +2586,13 @@
       <c r="A37" s="8">
         <v>11</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
       <c r="I37" s="11">
         <v>9</v>
       </c>
@@ -1962,433 +2601,849 @@
       <c r="A38" s="9">
         <v>12</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
       <c r="I38" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="16.8" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="28" t="s">
+    <row r="50" spans="1:12" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="1:12" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="30" t="s">
+      <c r="B51" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="29" t="s">
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="A52" s="8">
         <v>1</v>
       </c>
       <c r="B52" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="26"/>
-      <c r="K52" s="26"/>
-      <c r="L52" s="29" t="s">
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="26">
+      <c r="A53" s="34">
         <v>2</v>
       </c>
-      <c r="B53" s="26"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="26"/>
-      <c r="K53" s="26"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
       <c r="L53" s="30" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="26"/>
-      <c r="K54" s="26"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
       <c r="L54" s="30"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="26"/>
-      <c r="K55" s="26"/>
-      <c r="L55" s="29"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28"/>
+      <c r="J55" s="28"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="20"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="A56" s="8">
         <v>3</v>
       </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="26"/>
-      <c r="I56" s="26"/>
-      <c r="J56" s="26"/>
-      <c r="K56" s="26"/>
-      <c r="L56" s="29">
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+      <c r="J56" s="28"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="20">
         <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="A57" s="8">
         <v>4</v>
       </c>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="26"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
-      <c r="K57" s="26"/>
-      <c r="L57" s="29">
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="20">
         <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="A58" s="8">
         <v>5</v>
       </c>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
-      <c r="K58" s="26"/>
-      <c r="L58" s="29">
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="28"/>
+      <c r="J58" s="28"/>
+      <c r="K58" s="28"/>
+      <c r="L58" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="26"/>
-      <c r="K59" s="26"/>
-      <c r="L59" s="29"/>
+      <c r="A59" s="8"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="28"/>
+      <c r="I59" s="28"/>
+      <c r="J59" s="28"/>
+      <c r="K59" s="28"/>
+      <c r="L59" s="20"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="A60" s="8">
         <v>6</v>
       </c>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="26"/>
-      <c r="I60" s="26"/>
-      <c r="J60" s="26"/>
-      <c r="K60" s="26"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="28"/>
+      <c r="I60" s="28"/>
+      <c r="J60" s="28"/>
+      <c r="K60" s="28"/>
       <c r="L60" s="30">
         <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="A61" s="8">
         <v>7</v>
       </c>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
-      <c r="K61" s="26"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="28"/>
+      <c r="I61" s="28"/>
+      <c r="J61" s="28"/>
+      <c r="K61" s="28"/>
       <c r="L61" s="30"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="A62" s="8">
         <v>8</v>
       </c>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
-      <c r="I62" s="26"/>
-      <c r="J62" s="26"/>
-      <c r="K62" s="26"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="28"/>
+      <c r="K62" s="28"/>
       <c r="L62" s="30"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63">
+      <c r="A63" s="8">
         <v>9</v>
       </c>
-      <c r="B63" s="26"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="26"/>
-      <c r="I63" s="26"/>
-      <c r="J63" s="26"/>
-      <c r="K63" s="26"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="28"/>
+      <c r="J63" s="28"/>
+      <c r="K63" s="28"/>
       <c r="L63" s="30"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64">
+      <c r="A64" s="8">
         <v>10</v>
       </c>
-      <c r="B64" s="26"/>
-      <c r="C64" s="26"/>
-      <c r="D64" s="26"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="26"/>
-      <c r="G64" s="26"/>
-      <c r="H64" s="26"/>
-      <c r="I64" s="26"/>
-      <c r="J64" s="26"/>
-      <c r="K64" s="26"/>
-      <c r="L64" s="29">
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="28"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="28"/>
+      <c r="K64" s="28"/>
+      <c r="L64" s="20">
         <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65">
+      <c r="A65" s="8">
         <v>11</v>
       </c>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="26"/>
-      <c r="G65" s="26"/>
-      <c r="H65" s="26"/>
-      <c r="I65" s="26"/>
-      <c r="J65" s="26"/>
-      <c r="K65" s="26"/>
-      <c r="L65" s="29">
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+      <c r="J65" s="28"/>
+      <c r="K65" s="28"/>
+      <c r="L65" s="20">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66">
+    <row r="66" spans="1:12" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="9">
         <v>12</v>
       </c>
-      <c r="B66" s="26"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="26"/>
-      <c r="G66" s="26"/>
-      <c r="H66" s="26"/>
-      <c r="I66" s="26"/>
-      <c r="J66" s="26"/>
-      <c r="K66" s="26"/>
-      <c r="L66" s="29">
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="29"/>
+      <c r="K66" s="29"/>
+      <c r="L66" s="12">
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="28" t="s">
+    <row r="67" spans="1:12" ht="16.8" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:12" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="81" spans="1:9" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B81" s="30" t="s">
+      <c r="B81" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
-      <c r="E81" s="30"/>
-      <c r="F81" s="30"/>
-      <c r="G81" s="30"/>
-      <c r="H81" s="30"/>
-      <c r="I81" s="29" t="s">
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="26"/>
+      <c r="H81" s="26"/>
+      <c r="I81" s="10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82">
+      <c r="A82" s="8">
         <v>1</v>
       </c>
       <c r="B82" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C82" s="26"/>
-      <c r="D82" s="26"/>
-      <c r="E82" s="26"/>
-      <c r="F82" s="26"/>
-      <c r="G82" s="26"/>
-      <c r="H82" s="26"/>
-      <c r="I82" s="29">
+      <c r="C82" s="28"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="28"/>
+      <c r="F82" s="28"/>
+      <c r="G82" s="28"/>
+      <c r="H82" s="28"/>
+      <c r="I82" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83">
+      <c r="A83" s="8">
         <v>2</v>
       </c>
-      <c r="B83" s="26"/>
-      <c r="C83" s="26"/>
-      <c r="D83" s="26"/>
-      <c r="E83" s="26"/>
-      <c r="F83" s="26"/>
-      <c r="G83" s="26"/>
-      <c r="H83" s="26"/>
-      <c r="I83" s="29">
+      <c r="B83" s="28"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="28"/>
+      <c r="G83" s="28"/>
+      <c r="H83" s="28"/>
+      <c r="I83" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84">
+      <c r="A84" s="8">
         <v>3</v>
       </c>
-      <c r="B84" s="26"/>
-      <c r="C84" s="26"/>
-      <c r="D84" s="26"/>
-      <c r="E84" s="26"/>
-      <c r="F84" s="26"/>
-      <c r="G84" s="26"/>
-      <c r="H84" s="26"/>
-      <c r="I84" s="29"/>
+      <c r="B84" s="28"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="28"/>
+      <c r="G84" s="28"/>
+      <c r="H84" s="28"/>
+      <c r="I84" s="20"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85">
+      <c r="A85" s="8">
         <v>4</v>
       </c>
-      <c r="B85" s="26"/>
-      <c r="C85" s="26"/>
-      <c r="D85" s="26"/>
-      <c r="E85" s="26"/>
-      <c r="F85" s="26"/>
-      <c r="G85" s="26"/>
-      <c r="H85" s="26"/>
-      <c r="I85" s="29">
+      <c r="B85" s="28"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="28"/>
+      <c r="F85" s="28"/>
+      <c r="G85" s="28"/>
+      <c r="H85" s="28"/>
+      <c r="I85" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86">
+      <c r="A86" s="8">
         <v>5</v>
       </c>
-      <c r="B86" s="26"/>
-      <c r="C86" s="26"/>
-      <c r="D86" s="26"/>
-      <c r="E86" s="26"/>
-      <c r="F86" s="26"/>
-      <c r="G86" s="26"/>
-      <c r="H86" s="26"/>
-      <c r="I86" s="29" t="s">
+      <c r="B86" s="28"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="28"/>
+      <c r="F86" s="28"/>
+      <c r="G86" s="28"/>
+      <c r="H86" s="28"/>
+      <c r="I86" s="20" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87">
+      <c r="A87" s="8">
         <v>6</v>
       </c>
-      <c r="B87" s="26"/>
-      <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
-      <c r="F87" s="26"/>
-      <c r="G87" s="26"/>
-      <c r="H87" s="26"/>
-      <c r="I87" s="29" t="s">
+      <c r="B87" s="28"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="28"/>
+      <c r="F87" s="28"/>
+      <c r="G87" s="28"/>
+      <c r="H87" s="28"/>
+      <c r="I87" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88">
+      <c r="A88" s="8">
         <v>7</v>
       </c>
-      <c r="B88" s="26"/>
-      <c r="C88" s="26"/>
-      <c r="D88" s="26"/>
-      <c r="E88" s="26"/>
-      <c r="F88" s="26"/>
-      <c r="G88" s="26"/>
-      <c r="H88" s="26"/>
-      <c r="I88" s="29">
+      <c r="B88" s="28"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="28"/>
+      <c r="H88" s="28"/>
+      <c r="I88" s="20">
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89">
+    <row r="89" spans="1:9" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="9">
         <v>8</v>
       </c>
-      <c r="B89" s="26"/>
-      <c r="C89" s="26"/>
-      <c r="D89" s="26"/>
-      <c r="E89" s="26"/>
-      <c r="F89" s="26"/>
-      <c r="G89" s="26"/>
-      <c r="H89" s="26"/>
-      <c r="I89" s="29"/>
-    </row>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="29"/>
+      <c r="G89" s="29"/>
+      <c r="H89" s="29"/>
+      <c r="I89" s="12"/>
+    </row>
+    <row r="90" spans="1:9" ht="16.8" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="111" spans="1:10" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B111" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C111" s="26"/>
+      <c r="D111" s="26"/>
+      <c r="E111" s="26"/>
+      <c r="F111" s="26"/>
+      <c r="G111" s="26"/>
+      <c r="H111" s="26"/>
+      <c r="I111" s="26"/>
+      <c r="J111" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A112" s="8">
+        <v>1</v>
+      </c>
+      <c r="B112" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C112" s="28"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="28"/>
+      <c r="F112" s="28"/>
+      <c r="G112" s="28"/>
+      <c r="H112" s="28"/>
+      <c r="I112" s="28"/>
+      <c r="J112" s="20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A113" s="34">
+        <v>2</v>
+      </c>
+      <c r="B113" s="28"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="28"/>
+      <c r="E113" s="28"/>
+      <c r="F113" s="28"/>
+      <c r="G113" s="28"/>
+      <c r="H113" s="28"/>
+      <c r="I113" s="28"/>
+      <c r="J113" s="30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A114" s="34"/>
+      <c r="B114" s="28"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="28"/>
+      <c r="F114" s="28"/>
+      <c r="G114" s="28"/>
+      <c r="H114" s="28"/>
+      <c r="I114" s="28"/>
+      <c r="J114" s="30"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A115" s="8">
+        <v>3</v>
+      </c>
+      <c r="B115" s="28"/>
+      <c r="C115" s="28"/>
+      <c r="D115" s="28"/>
+      <c r="E115" s="28"/>
+      <c r="F115" s="28"/>
+      <c r="G115" s="28"/>
+      <c r="H115" s="28"/>
+      <c r="I115" s="28"/>
+      <c r="J115" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A116" s="8"/>
+      <c r="B116" s="28"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="28"/>
+      <c r="E116" s="28"/>
+      <c r="F116" s="28"/>
+      <c r="G116" s="28"/>
+      <c r="H116" s="28"/>
+      <c r="I116" s="28"/>
+      <c r="J116" s="20"/>
+    </row>
+    <row r="117" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="9">
+        <v>4</v>
+      </c>
+      <c r="B117" s="29"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+      <c r="G117" s="29"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="29"/>
+      <c r="J117" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="16.8" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="131" spans="1:10" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B131" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C131" s="26"/>
+      <c r="D131" s="26"/>
+      <c r="E131" s="26"/>
+      <c r="F131" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A132" s="8">
+        <v>1</v>
+      </c>
+      <c r="B132" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C132" s="28"/>
+      <c r="D132" s="28"/>
+      <c r="E132" s="28"/>
+      <c r="F132" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A133" s="8">
+        <v>2</v>
+      </c>
+      <c r="B133" s="28"/>
+      <c r="C133" s="28"/>
+      <c r="D133" s="28"/>
+      <c r="E133" s="28"/>
+      <c r="F133" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A134" s="8">
+        <v>3</v>
+      </c>
+      <c r="B134" s="28"/>
+      <c r="C134" s="28"/>
+      <c r="D134" s="28"/>
+      <c r="E134" s="28"/>
+      <c r="F134" s="20"/>
+    </row>
+    <row r="135" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A135" s="9">
+        <v>4</v>
+      </c>
+      <c r="B135" s="29"/>
+      <c r="C135" s="29"/>
+      <c r="D135" s="29"/>
+      <c r="E135" s="29"/>
+      <c r="F135" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="16.8" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="140" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="141" spans="1:10" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B141" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C141" s="26"/>
+      <c r="D141" s="26"/>
+      <c r="E141" s="26"/>
+      <c r="F141" s="26"/>
+      <c r="G141" s="26"/>
+      <c r="H141" s="26"/>
+      <c r="I141" s="26"/>
+      <c r="J141" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A142" s="8">
+        <v>1</v>
+      </c>
+      <c r="B142" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C142" s="28"/>
+      <c r="D142" s="28"/>
+      <c r="E142" s="28"/>
+      <c r="F142" s="28"/>
+      <c r="G142" s="28"/>
+      <c r="H142" s="28"/>
+      <c r="I142" s="28"/>
+      <c r="J142" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A143" s="8">
+        <v>2</v>
+      </c>
+      <c r="B143" s="28"/>
+      <c r="C143" s="28"/>
+      <c r="D143" s="28"/>
+      <c r="E143" s="28"/>
+      <c r="F143" s="28"/>
+      <c r="G143" s="28"/>
+      <c r="H143" s="28"/>
+      <c r="I143" s="28"/>
+      <c r="J143" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A144" s="8">
+        <v>3</v>
+      </c>
+      <c r="B144" s="28"/>
+      <c r="C144" s="28"/>
+      <c r="D144" s="28"/>
+      <c r="E144" s="28"/>
+      <c r="F144" s="28"/>
+      <c r="G144" s="28"/>
+      <c r="H144" s="28"/>
+      <c r="I144" s="28"/>
+      <c r="J144" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A145" s="8">
+        <v>4</v>
+      </c>
+      <c r="B145" s="28"/>
+      <c r="C145" s="28"/>
+      <c r="D145" s="28"/>
+      <c r="E145" s="28"/>
+      <c r="F145" s="28"/>
+      <c r="G145" s="28"/>
+      <c r="H145" s="28"/>
+      <c r="I145" s="28"/>
+      <c r="J145" s="20"/>
+    </row>
+    <row r="146" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="9">
+        <v>5</v>
+      </c>
+      <c r="B146" s="29"/>
+      <c r="C146" s="29"/>
+      <c r="D146" s="29"/>
+      <c r="E146" s="29"/>
+      <c r="F146" s="29"/>
+      <c r="G146" s="29"/>
+      <c r="H146" s="29"/>
+      <c r="I146" s="29"/>
+      <c r="J146" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" ht="16.8" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="155" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="156" spans="1:10" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B156" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C156" s="26"/>
+      <c r="D156" s="26"/>
+      <c r="E156" s="26"/>
+      <c r="F156" s="26"/>
+      <c r="G156" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A157" s="8">
+        <v>1</v>
+      </c>
+      <c r="B157" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C157" s="28"/>
+      <c r="D157" s="28"/>
+      <c r="E157" s="28"/>
+      <c r="F157" s="28"/>
+      <c r="G157" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A158" s="8">
+        <v>2</v>
+      </c>
+      <c r="B158" s="28"/>
+      <c r="C158" s="28"/>
+      <c r="D158" s="28"/>
+      <c r="E158" s="28"/>
+      <c r="F158" s="28"/>
+      <c r="G158" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A159" s="8">
+        <v>3</v>
+      </c>
+      <c r="B159" s="28"/>
+      <c r="C159" s="28"/>
+      <c r="D159" s="28"/>
+      <c r="E159" s="28"/>
+      <c r="F159" s="28"/>
+      <c r="G159" s="30"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A160" s="8">
+        <v>4</v>
+      </c>
+      <c r="B160" s="28"/>
+      <c r="C160" s="28"/>
+      <c r="D160" s="28"/>
+      <c r="E160" s="28"/>
+      <c r="F160" s="28"/>
+      <c r="G160" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A161" s="8">
+        <v>5</v>
+      </c>
+      <c r="B161" s="28"/>
+      <c r="C161" s="28"/>
+      <c r="D161" s="28"/>
+      <c r="E161" s="28"/>
+      <c r="F161" s="28"/>
+      <c r="G161" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A162" s="8">
+        <v>6</v>
+      </c>
+      <c r="B162" s="28"/>
+      <c r="C162" s="28"/>
+      <c r="D162" s="28"/>
+      <c r="E162" s="28"/>
+      <c r="F162" s="28"/>
+      <c r="G162" s="30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A163" s="8">
+        <v>7</v>
+      </c>
+      <c r="B163" s="28"/>
+      <c r="C163" s="28"/>
+      <c r="D163" s="28"/>
+      <c r="E163" s="28"/>
+      <c r="F163" s="28"/>
+      <c r="G163" s="30"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A164" s="8">
+        <v>8</v>
+      </c>
+      <c r="B164" s="28"/>
+      <c r="C164" s="28"/>
+      <c r="D164" s="28"/>
+      <c r="E164" s="28"/>
+      <c r="F164" s="28"/>
+      <c r="G164" s="20"/>
+    </row>
+    <row r="165" spans="1:7" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="9">
+        <v>9</v>
+      </c>
+      <c r="B165" s="29"/>
+      <c r="C165" s="29"/>
+      <c r="D165" s="29"/>
+      <c r="E165" s="29"/>
+      <c r="F165" s="29"/>
+      <c r="G165" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="16.8" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B82:H89"/>
-    <mergeCell ref="B81:H81"/>
-    <mergeCell ref="B52:K66"/>
-    <mergeCell ref="L53:L54"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="L60:L63"/>
+  <mergeCells count="28">
+    <mergeCell ref="B142:I146"/>
+    <mergeCell ref="B141:I141"/>
+    <mergeCell ref="B157:F165"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="G158:G159"/>
+    <mergeCell ref="G162:G163"/>
+    <mergeCell ref="B112:I117"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="J113:J114"/>
+    <mergeCell ref="B111:I111"/>
+    <mergeCell ref="B132:E135"/>
+    <mergeCell ref="B131:E131"/>
     <mergeCell ref="B51:K51"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B27:H38"/>
@@ -2399,6 +3454,12 @@
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="I8:I10"/>
     <mergeCell ref="I11:I13"/>
+    <mergeCell ref="B82:H89"/>
+    <mergeCell ref="B81:H81"/>
+    <mergeCell ref="B52:K66"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="L60:L63"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>